<commit_message>
commit actualizar sptrin 2 excel Estimacion de Esfuerzo
</commit_message>
<xml_diff>
--- a/Gestión/Estimacion de Esfuerzo_TB (1).xlsx
+++ b/Gestión/Estimacion de Esfuerzo_TB (1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brayan Muñoz\Desktop\Documents\UPC\Ciclo 7\Evolución de Software\Trabajo\Semana 6 - 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brayan Muñoz\Documents\GitHub\AndroidSuperMarket\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -614,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -711,6 +711,13 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1345,7 +1352,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Estimacion de Esfuerzo_TB.xlsx]SPRINT_PROYECTO!Tabla dinámica2</c:name>
+    <c:name>[Estimacion de Esfuerzo_TB (1).xlsx]SPRINT_PROYECTO!Tabla dinámica2</c:name>
     <c:fmtId val="4"/>
   </c:pivotSource>
   <c:chart>
@@ -1854,12 +1861,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="179499600"/>
-        <c:axId val="179496880"/>
+        <c:axId val="972395616"/>
+        <c:axId val="972397248"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="179499600"/>
+        <c:axId val="972395616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1902,7 +1909,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179496880"/>
+        <c:crossAx val="972397248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1910,7 +1917,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="179496880"/>
+        <c:axId val="972397248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1960,7 +1967,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179499600"/>
+        <c:crossAx val="972395616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1974,6 +1981,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3648,8 +3656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3894,7 +3902,7 @@
         <f>IFERROR(VLOOKUP(Tabla2[[#This Row],[IM01]],TABLA_ESTIMADOS,13,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM02]],TABLA_ESTIMADOS,14,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM03]],TABLA_ESTIMADOS,15,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM04]],TABLA_ESTIMADOS,16,FALSE),0)</f>
         <v>9</v>
       </c>
-      <c r="U5" s="20">
+      <c r="U5" s="38">
         <f>+Tabla2[[#This Row],[IM00]]+Tabla2[[#This Row],[PR00]]+Tabla2[[#This Row],[DI00]]+Tabla2[[#This Row],[RQ00]]</f>
         <v>19.5</v>
       </c>
@@ -3904,7 +3912,7 @@
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>61</v>
@@ -3975,7 +3983,7 @@
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>60</v>
@@ -4107,7 +4115,7 @@
         <f>IFERROR(VLOOKUP(Tabla2[[#This Row],[IM01]],TABLA_ESTIMADOS,13,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM02]],TABLA_ESTIMADOS,14,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM03]],TABLA_ESTIMADOS,15,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM04]],TABLA_ESTIMADOS,16,FALSE),0)</f>
         <v>11</v>
       </c>
-      <c r="U8" s="20">
+      <c r="U8" s="38">
         <f>+Tabla2[[#This Row],[IM00]]+Tabla2[[#This Row],[PR00]]+Tabla2[[#This Row],[DI00]]+Tabla2[[#This Row],[RQ00]]</f>
         <v>24</v>
       </c>
@@ -4179,7 +4187,7 @@
         <f>IFERROR(VLOOKUP(Tabla2[[#This Row],[IM01]],TABLA_ESTIMADOS,13,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM02]],TABLA_ESTIMADOS,14,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM03]],TABLA_ESTIMADOS,15,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM04]],TABLA_ESTIMADOS,16,FALSE),0)</f>
         <v>11</v>
       </c>
-      <c r="U9" s="25">
+      <c r="U9" s="39">
         <f>+Tabla2[[#This Row],[IM00]]+Tabla2[[#This Row],[PR00]]+Tabla2[[#This Row],[DI00]]+Tabla2[[#This Row],[RQ00]]</f>
         <v>24</v>
       </c>
@@ -4250,7 +4258,7 @@
         <f>IFERROR(VLOOKUP(Tabla2[[#This Row],[IM01]],TABLA_ESTIMADOS,13,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM02]],TABLA_ESTIMADOS,14,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM03]],TABLA_ESTIMADOS,15,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM04]],TABLA_ESTIMADOS,16,FALSE),0)</f>
         <v>11</v>
       </c>
-      <c r="U10" s="25">
+      <c r="U10" s="39">
         <f>+Tabla2[[#This Row],[IM00]]+Tabla2[[#This Row],[PR00]]+Tabla2[[#This Row],[DI00]]+Tabla2[[#This Row],[RQ00]]</f>
         <v>24</v>
       </c>
@@ -4534,13 +4542,16 @@
         <f>IFERROR(VLOOKUP(Tabla2[[#This Row],[IM01]],TABLA_ESTIMADOS,13,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM02]],TABLA_ESTIMADOS,14,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM03]],TABLA_ESTIMADOS,15,FALSE),0)+IFERROR(VLOOKUP(Tabla2[[#This Row],[IM04]],TABLA_ESTIMADOS,16,FALSE),0)</f>
         <v>9</v>
       </c>
-      <c r="U14" s="20">
+      <c r="U14" s="38">
         <f>+Tabla2[[#This Row],[IM00]]+Tabla2[[#This Row],[PR00]]+Tabla2[[#This Row],[DI00]]+Tabla2[[#This Row],[RQ00]]</f>
         <v>19.5</v>
       </c>
       <c r="V14" s="6">
         <v>0.13</v>
       </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="U16" s="37"/>
     </row>
     <row r="20" spans="4:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="4:20" x14ac:dyDescent="0.2">

</xml_diff>